<commit_message>
Change file / directory
</commit_message>
<xml_diff>
--- a/原始金融服务网鱼原始凭证.xlsx
+++ b/原始金融服务网鱼原始凭证.xlsx
@@ -236,7 +236,7 @@
     <numFmt numFmtId="182" formatCode="00\ &quot;年&quot;"/>
     <numFmt numFmtId="183" formatCode="&quot;¥&quot;\ #,##0.00;\(&quot;¥&quot;\ #,##0.00\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,7 +657,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.25" style="1" bestFit="1" customWidth="1"/>
@@ -665,7 +665,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -682,12 +682,12 @@
         <v>26</v>
       </c>
       <c r="F1" s="19">
-        <v>89.73</v>
+        <v>85.36</v>
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -696,7 +696,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -713,7 +713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
@@ -730,7 +730,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -750,7 +750,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -770,7 +770,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
@@ -790,7 +790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>34</v>
@@ -811,7 +811,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -831,7 +831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -854,12 +854,12 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="17">
-        <v>45454.382789351854</v>
+        <v>45459.331296296295</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -867,7 +867,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -881,22 +881,22 @@
         <v>0</v>
       </c>
       <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11">
+        <v>40</v>
+      </c>
+      <c r="G15" s="12">
         <v>0</v>
       </c>
-      <c r="F15" s="11">
-        <v>21</v>
-      </c>
-      <c r="G15" s="12">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>CONCATENATE(TEXT(DATE(YEAR(上机时间)+上机时长_年,MONTH(上机时间)+上机时长_月,DAY(上机时间)+上机时长_日),"yyyy-mm-dd")," ",TEXT(TIME(HOUR(上机时间)+上机时长_时,MINUTE(上机时间)+上机时长_分,SECOND(上机时间)+上机时长_秒),"hh:mm:ss"))</f>
-        <v>2024-06-11 09:33:12</v>
+        <v>2024-06-16 09:37:04</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -904,54 +904,54 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="4">
         <f>TEXT(下机时间-上机时间,"[ss]")/3600*区域费率+服务费率</f>
-        <v>1.5655555555555556</v>
+        <v>6.7666666666666666</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="4">
         <f>上网费用*服务费率</f>
-        <v>0.15655555555555556</v>
+        <v>0.67666666666666675</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="14">
         <f>-(上网费用-(上网费用*鱼乐卡折扣))</f>
-        <v>-7.827777777777789E-2</v>
+        <v>-0.33833333333333382</v>
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="19">
         <f>上网费用+平台服务费+鱼乐卡权益</f>
-        <v>1.6438333333333333</v>
+        <v>7.1049999999999995</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="19">
         <f>总金额-本次消费</f>
-        <v>88.086166666666671</v>
+        <v>78.254999999999995</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
+    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="5"/>
     </row>
   </sheetData>
@@ -982,7 +982,7 @@
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.25" style="1" bestFit="1" customWidth="1"/>
@@ -990,7 +990,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1007,12 +1007,12 @@
         <v>26</v>
       </c>
       <c r="F1" s="19">
-        <v>89.73</v>
+        <v>85.36</v>
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" thickTop="1"/>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>34</v>
@@ -1136,8 +1136,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1"/>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="D12" s="2">
         <f>IF(OR(WEEKDAY(下机时间)-1=5,WEEKDAY(下机时间)-1=6,WEEKDAY(下机时间)-1=0),IF(鱼乐卡等级="普通",HLOOKUP(区域类型,C6:G9,2,0),HLOOKUP(区域类型,C6:G9,4,0)),IF(鱼乐卡等级="普通",HLOOKUP(区域类型,C6:G9,2,0),HLOOKUP(区域类型,C6:G9,3,0)))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>32</v>
@@ -1180,13 +1180,13 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1"/>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="17">
-        <v>45454.382789351854</v>
+        <v>45459.331296296295</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -1194,7 +1194,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1208,22 +1208,22 @@
         <v>0</v>
       </c>
       <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11">
+        <v>40</v>
+      </c>
+      <c r="G15" s="12">
         <v>0</v>
       </c>
-      <c r="F15" s="11">
-        <v>21</v>
-      </c>
-      <c r="G15" s="12">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>CONCATENATE(TEXT(DATE(YEAR(上机时间)+上机时长_年,MONTH(上机时间)+上机时长_月,DAY(上机时间)+上机时长_日),"yyyy-mm-dd")," ",TEXT(TIME(HOUR(上机时间)+上机时长_时,MINUTE(上机时间)+上机时长_分,SECOND(上机时间)+上机时长_秒),"hh:mm:ss"))</f>
-        <v>2024-06-11 09:33:12</v>
+        <v>2024-06-16 09:37:04</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1231,54 +1231,54 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="4">
         <f>TEXT(下机时间-上机时间,"[ss]")/3600*区域费率+服务费率</f>
-        <v>2.2983333333333333</v>
+        <v>11.766666666666667</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="4">
         <f>上网费用*服务费率</f>
-        <v>0.22983333333333333</v>
+        <v>1.1766666666666667</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F18" s="14">
         <f>-(上网费用-(上网费用*鱼乐卡折扣))</f>
-        <v>-0.11491666666666678</v>
+        <v>-0.58833333333333471</v>
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="19">
         <f>上网费用+平台服务费+鱼乐卡权益</f>
-        <v>2.4132499999999997</v>
+        <v>12.355</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="19">
         <f>总金额-本次消费</f>
-        <v>87.316749999999999</v>
+        <v>73.004999999999995</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" thickTop="1"/>
+    <row r="21" spans="1:7">
       <c r="B21" s="5"/>
     </row>
   </sheetData>

</xml_diff>